<commit_message>
added some text to federal revenue page
</commit_message>
<xml_diff>
--- a/fedCUREexpenditures.xlsx
+++ b/fedCUREexpenditures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures FY2022\Fiscal-Future-Topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6771A95C-CA1C-47F3-AC8E-5B135A2FAF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3328BC75-46A7-4381-B48D-F961536145A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1800" windowWidth="17280" windowHeight="8994" xr2:uid="{BD32768A-AB64-44D0-96D5-D68339992D9F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{BD32768A-AB64-44D0-96D5-D68339992D9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="72">
   <si>
     <t>Federal Funds</t>
   </si>
@@ -137,27 +137,18 @@
     <t>Employment and Training Fund</t>
   </si>
   <si>
-    <t>CRRSA/ARPA</t>
-  </si>
-  <si>
     <t>Child Care Development Block Grant</t>
   </si>
   <si>
     <t>Child Care Stabilization Grants</t>
   </si>
   <si>
-    <t>Child Care Entitlement to States</t>
-  </si>
-  <si>
     <t>Public Health</t>
   </si>
   <si>
     <t>Public Health Services</t>
   </si>
   <si>
-    <t>CARES/ARPA</t>
-  </si>
-  <si>
     <t>Health Protection and Lab Capacity</t>
   </si>
   <si>
@@ -179,9 +170,6 @@
     <t>UI Trust Fund</t>
   </si>
   <si>
-    <t>Excluded</t>
-  </si>
-  <si>
     <t>Other Fed Rev</t>
   </si>
   <si>
@@ -221,18 +209,6 @@
     <t>LIHEAP</t>
   </si>
   <si>
-    <t>DOR</t>
-  </si>
-  <si>
-    <t>Covid19 Housing Grant Program - Reappropriation</t>
-  </si>
-  <si>
-    <t>COVID Housing Grant Program</t>
-  </si>
-  <si>
-    <t>Support for Long-term Care providers</t>
-  </si>
-  <si>
     <t>Econ Dev</t>
   </si>
   <si>
@@ -243,6 +219,39 @@
   </si>
   <si>
     <t>FY_Received</t>
+  </si>
+  <si>
+    <t>Not used - Full Expenditures(NotjustCOVID fed $)</t>
+  </si>
+  <si>
+    <t>Rev_FY</t>
+  </si>
+  <si>
+    <t>Rev_$</t>
+  </si>
+  <si>
+    <t>FY22</t>
+  </si>
+  <si>
+    <t>FY21</t>
+  </si>
+  <si>
+    <t>ESER 1</t>
+  </si>
+  <si>
+    <t>Formula funding to states to from the CARES Act to respond to school closures, meet student &amp; teacher needs, &amp; improve technology.</t>
+  </si>
+  <si>
+    <t>UI Fund</t>
+  </si>
+  <si>
+    <t>2023+</t>
+  </si>
+  <si>
+    <t>Appropriated and partially spent</t>
+  </si>
+  <si>
+    <t>FY23+</t>
   </si>
 </sst>
 </file>
@@ -283,9 +292,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,24 +612,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26519E7A-CD6D-4FF8-AA8F-CD3C7AE7805F}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="5" max="5" width="23.69921875" customWidth="1"/>
     <col min="7" max="7" width="37.046875" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" customWidth="1"/>
+    <col min="14" max="14" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -638,18 +652,27 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C2">
         <v>2021</v>
@@ -669,19 +692,20 @@
       <c r="H2" s="1">
         <v>132</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1"/>
+      <c r="J2">
         <v>1.8</v>
       </c>
-      <c r="J2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C3">
         <v>2021</v>
@@ -701,19 +725,20 @@
       <c r="H3" s="1">
         <v>322</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1"/>
+      <c r="J3">
         <v>1.8</v>
       </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C4">
         <v>2021</v>
@@ -733,19 +758,20 @@
       <c r="H4" s="1">
         <v>260</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1"/>
+      <c r="J4">
         <v>1.8</v>
       </c>
-      <c r="J4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C5">
         <v>2021</v>
@@ -765,16 +791,16 @@
       <c r="H5">
         <v>240</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C6">
         <v>2021</v>
@@ -794,16 +820,16 @@
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="J6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C7">
         <v>2021</v>
@@ -823,19 +849,20 @@
       <c r="H7" s="1">
         <v>337</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1"/>
+      <c r="J7">
         <v>1.8</v>
       </c>
-      <c r="J7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C8">
         <v>2021</v>
@@ -855,19 +882,20 @@
       <c r="H8" s="1">
         <v>30</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1"/>
+      <c r="J8">
         <v>1.8</v>
       </c>
-      <c r="J8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C9">
         <v>2021</v>
@@ -887,19 +915,20 @@
       <c r="H9" s="1">
         <v>30</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1"/>
+      <c r="J9">
         <v>1.8</v>
       </c>
-      <c r="J9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C10">
         <v>2021</v>
@@ -919,19 +948,20 @@
       <c r="H10" s="1">
         <v>705</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1"/>
+      <c r="J10">
         <v>1.8</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C11">
         <v>2021</v>
@@ -951,11 +981,11 @@
       <c r="H11">
         <v>295</v>
       </c>
-      <c r="J11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -972,24 +1002,24 @@
         <v>32</v>
       </c>
       <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" t="s">
         <v>33</v>
       </c>
-      <c r="G12" t="s">
-        <v>34</v>
-      </c>
       <c r="H12">
-        <v>775</v>
-      </c>
-      <c r="J12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>332</v>
+      </c>
+      <c r="K12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C13">
         <v>2022</v>
@@ -1004,21 +1034,21 @@
         <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H13">
-        <v>501</v>
-      </c>
-      <c r="J13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>775</v>
+      </c>
+      <c r="K13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C14">
         <v>2022</v>
@@ -1033,45 +1063,45 @@
         <v>31</v>
       </c>
       <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14">
+        <v>501</v>
+      </c>
+      <c r="K14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>2021</v>
+      </c>
+      <c r="C15">
+        <v>2022</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
         <v>36</v>
       </c>
-      <c r="H14">
-        <v>775</v>
-      </c>
-      <c r="J14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15">
-        <v>2020</v>
-      </c>
-      <c r="C15">
-        <v>2022</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
         <v>37</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" t="s">
-        <v>40</v>
       </c>
       <c r="H15">
         <v>267</v>
       </c>
-      <c r="J15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1081,23 +1111,26 @@
       <c r="C16">
         <v>2022</v>
       </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F16" t="s">
         <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H16">
         <v>175</v>
       </c>
-      <c r="J16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1111,111 +1144,123 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
         <v>31</v>
       </c>
       <c r="G17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H17">
         <v>115</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>2022</v>
+      </c>
+      <c r="C18">
+        <v>2022</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18">
-        <v>2022</v>
-      </c>
-      <c r="C18">
-        <v>2022</v>
-      </c>
-      <c r="D18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" t="s">
-        <v>45</v>
       </c>
       <c r="F18" t="s">
         <v>31</v>
       </c>
       <c r="G18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H18">
         <v>2700</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
+        <v>68</v>
+      </c>
+      <c r="M18" t="s">
+        <v>65</v>
+      </c>
+      <c r="N18">
+        <v>677964975</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19">
+        <v>2021</v>
+      </c>
+      <c r="C19">
+        <v>2022</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19">
-        <v>2021</v>
-      </c>
-      <c r="C19">
-        <v>2022</v>
-      </c>
-      <c r="D19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" t="s">
-        <v>51</v>
-      </c>
       <c r="G19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H19">
         <v>906</v>
       </c>
-      <c r="J19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K19" t="s">
+        <v>59</v>
+      </c>
+      <c r="M19" t="s">
+        <v>64</v>
+      </c>
+      <c r="N19">
+        <v>2250804891</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20">
+        <v>2022</v>
+      </c>
+      <c r="C20">
+        <v>2022</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
         <v>48</v>
-      </c>
-      <c r="B20">
-        <v>2022</v>
-      </c>
-      <c r="C20">
-        <v>2022</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" t="s">
-        <v>52</v>
       </c>
       <c r="F20" t="s">
         <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H20">
         <v>444</v>
       </c>
-      <c r="J20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B21">
         <v>2022</v>
@@ -1224,27 +1269,27 @@
         <v>2022</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
         <v>31</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H21">
         <v>210</v>
       </c>
-      <c r="J21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B22">
         <v>2022</v>
@@ -1253,27 +1298,27 @@
         <v>2022</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
         <v>31</v>
       </c>
       <c r="G22" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H22">
         <v>243</v>
       </c>
-      <c r="J22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B23">
         <v>2021</v>
@@ -1285,22 +1330,22 @@
         <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H23">
         <v>218</v>
       </c>
-      <c r="J23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1314,62 +1359,65 @@
         <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F24" t="s">
         <v>31</v>
       </c>
       <c r="G24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H24">
         <v>304</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25">
+        <v>2021</v>
+      </c>
+      <c r="C25">
+        <v>2022</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25">
+        <v>569.5</v>
+      </c>
+      <c r="K25" t="s">
+        <v>59</v>
+      </c>
+      <c r="M25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25">
-        <v>2022</v>
-      </c>
-      <c r="C25">
-        <v>2023</v>
-      </c>
-      <c r="D25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25">
-        <v>135</v>
-      </c>
-      <c r="J25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>9</v>
       </c>
       <c r="B26">
         <v>2022</v>
       </c>
-      <c r="C26">
-        <v>2023</v>
+      <c r="C26" t="s">
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
         <v>31</v>
@@ -1378,13 +1426,13 @@
         <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H26">
-        <v>104.1</v>
-      </c>
-      <c r="J26" t="s">
-        <v>37</v>
+        <v>3000</v>
+      </c>
+      <c r="K26" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>